<commit_message>
some changes in the official_marks_doc_a3_two_face.xlsx file
</commit_message>
<xml_diff>
--- a/telegram_bot/templet_files/official_marks_doc_a3_two_face.xlsx
+++ b/telegram_bot/templet_files/official_marks_doc_a3_two_face.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -620,7 +620,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,6 +871,18 @@
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3899,14 +3911,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>-512640</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>-80640</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>203040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>-506880</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>-33840</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
@@ -3916,12 +3928,14 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip r:embed="rId1">
+          <a:alphaModFix amt="95000"/>
+        </a:blip>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-11015640" y="507960"/>
+          <a:off x="-11771640" y="507960"/>
           <a:ext cx="5252400" cy="7353720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3936,16 +3950,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>-545040</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>-500760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>-429840</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>-103680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>264960</xdr:rowOff>
+      <xdr:rowOff>300960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3954,7 +3968,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-11048040" y="2504520"/>
+          <a:off x="-11588040" y="2540520"/>
           <a:ext cx="1998720" cy="427320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4001,14 +4015,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>-268200</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>-375120</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>53280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>-392400</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>-187560</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>251640</xdr:rowOff>
     </xdr:to>
@@ -4019,7 +4033,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9320760" y="4529880"/>
+          <a:off x="-9860760" y="4529880"/>
           <a:ext cx="1496880" cy="198360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4065,14 +4079,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>-279000</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>-133920</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>217800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>-616680</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-159840</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>43560</xdr:rowOff>
     </xdr:to>
@@ -4083,7 +4097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9764640" y="4694400"/>
+          <a:off x="-10052640" y="4694400"/>
           <a:ext cx="1716480" cy="187920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4129,14 +4143,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>-203760</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>-237600</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>318240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>-808200</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-17280</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
@@ -4147,7 +4161,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9256320" y="5518800"/>
+          <a:off x="-10156320" y="5518800"/>
           <a:ext cx="1962720" cy="452520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4203,16 +4217,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>-393120</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>330840</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>-320040</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>-430560</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-45720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>292320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4221,7 +4235,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9878760" y="5893560"/>
+          <a:off x="-10238760" y="5929560"/>
           <a:ext cx="2016720" cy="287280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4268,14 +4282,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>-365400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>-256320</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>234000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>-450720</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-29880</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>341640</xdr:rowOff>
     </xdr:to>
@@ -4286,7 +4300,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9851040" y="6158520"/>
+          <a:off x="-10175040" y="6158520"/>
           <a:ext cx="1968840" cy="469800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4333,14 +4347,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>-375120</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>-336960</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>281520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>-571680</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-453600</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>307440</xdr:rowOff>
     </xdr:to>
@@ -4351,7 +4365,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9427680" y="6568200"/>
+          <a:off x="-10255680" y="6568200"/>
           <a:ext cx="2370600" cy="387720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4398,14 +4412,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>-304560</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>-338400</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>165600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>-565560</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>-519480</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>318240</xdr:rowOff>
     </xdr:to>
@@ -4416,7 +4430,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-9357120" y="6814080"/>
+          <a:off x="-10257120" y="6814080"/>
           <a:ext cx="2306160" cy="514440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4895,8 +4909,8 @@
   </sheetPr>
   <dimension ref="A1:U705"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA62" activeCellId="0" sqref="AA62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X60" activeCellId="0" sqref="X60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29937,8 +29951,8 @@
   </sheetPr>
   <dimension ref="A1:AJ71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29955,10 +29969,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="1" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="1" width="7.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="36" min="19" style="1" width="7.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="37" style="63" width="7.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="64" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -29969,8 +29984,34 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
-    </row>
-    <row r="2" s="10" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+    </row>
+    <row r="2" s="64" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -29981,8 +30022,34 @@
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
-    </row>
-    <row r="3" s="10" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+    </row>
+    <row r="3" s="64" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -29993,6 +30060,32 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="39"/>
@@ -30018,7 +30111,7 @@
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
     </row>
-    <row r="6" s="9" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="65" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -30029,8 +30122,34 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39"/>
-    </row>
-    <row r="7" s="9" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+    </row>
+    <row r="7" s="65" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
@@ -30041,8 +30160,34 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
-    </row>
-    <row r="8" s="9" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+    </row>
+    <row r="8" s="65" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -30053,8 +30198,34 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
-    </row>
-    <row r="9" s="9" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+    </row>
+    <row r="9" s="65" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
@@ -30065,8 +30236,34 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
-    </row>
-    <row r="10" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+    </row>
+    <row r="10" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
@@ -30077,8 +30274,34 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
-    </row>
-    <row r="11" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+    </row>
+    <row r="11" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -30089,8 +30312,34 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
-    </row>
-    <row r="12" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+    </row>
+    <row r="12" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -30101,8 +30350,34 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
-    </row>
-    <row r="13" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+    </row>
+    <row r="13" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -30113,8 +30388,34 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
-    </row>
-    <row r="14" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+    </row>
+    <row r="14" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -30125,8 +30426,34 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
       <c r="J14" s="39"/>
-    </row>
-    <row r="15" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+    </row>
+    <row r="15" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -30137,8 +30464,34 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
-    </row>
-    <row r="16" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+    </row>
+    <row r="16" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -30149,8 +30502,34 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
       <c r="J16" s="39"/>
-    </row>
-    <row r="17" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+    </row>
+    <row r="17" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -30161,8 +30540,34 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="39"/>
-    </row>
-    <row r="18" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+    </row>
+    <row r="18" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -30173,8 +30578,34 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
       <c r="J18" s="39"/>
-    </row>
-    <row r="19" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+    </row>
+    <row r="19" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -30185,8 +30616,34 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
       <c r="J19" s="39"/>
-    </row>
-    <row r="20" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+    </row>
+    <row r="20" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
@@ -30197,8 +30654,34 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
       <c r="J20" s="39"/>
-    </row>
-    <row r="21" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+    </row>
+    <row r="21" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
@@ -30209,8 +30692,34 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
-    </row>
-    <row r="22" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+    </row>
+    <row r="22" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="39"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
@@ -30221,8 +30730,34 @@
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
-    </row>
-    <row r="23" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+    </row>
+    <row r="23" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="39"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -30233,8 +30768,34 @@
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
       <c r="J23" s="39"/>
-    </row>
-    <row r="24" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+    </row>
+    <row r="24" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="39"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -30245,8 +30806,34 @@
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
-    </row>
-    <row r="25" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+    </row>
+    <row r="25" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="39"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -30257,8 +30844,34 @@
       <c r="H25" s="39"/>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
-    </row>
-    <row r="26" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+    </row>
+    <row r="26" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="39"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -30269,920 +30882,1032 @@
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
-    </row>
-    <row r="27" s="9" customFormat="true" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+    </row>
+    <row r="27" s="65" customFormat="true" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="39"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
       <c r="E27" s="39"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="67"/>
-      <c r="N27" s="67"/>
-      <c r="O27" s="67"/>
-      <c r="P27" s="67"/>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="68"/>
-    </row>
-    <row r="28" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="70"/>
+      <c r="R27" s="71"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+    </row>
+    <row r="28" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="39"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
       <c r="E28" s="39"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="63"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="72"/>
-      <c r="O28" s="72"/>
-      <c r="P28" s="72"/>
-      <c r="Q28" s="72"/>
-      <c r="R28" s="73"/>
-      <c r="S28" s="72"/>
-    </row>
-    <row r="29" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="76"/>
+      <c r="S28" s="75"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+    </row>
+    <row r="29" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="39"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
       <c r="E29" s="39"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="72"/>
-      <c r="N29" s="72"/>
-      <c r="O29" s="72"/>
-      <c r="P29" s="72"/>
-      <c r="Q29" s="72"/>
-      <c r="R29" s="73"/>
-      <c r="S29" s="72"/>
-    </row>
-    <row r="30" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="73"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="76"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
+    </row>
+    <row r="30" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="39"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
       <c r="E30" s="39"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="63"/>
-      <c r="L30" s="63"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="72"/>
-      <c r="P30" s="72"/>
-      <c r="Q30" s="72"/>
-      <c r="R30" s="73"/>
-      <c r="S30" s="72"/>
-    </row>
-    <row r="31" s="9" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="75"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="76"/>
+      <c r="S30" s="75"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="9"/>
+      <c r="AJ30" s="9"/>
+    </row>
+    <row r="31" s="65" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="39"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
       <c r="E31" s="39"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="63"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="76"/>
-      <c r="S32" s="74"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="79"/>
+      <c r="S32" s="77"/>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="76"/>
-      <c r="S33" s="74"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="77"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="77"/>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="74"/>
-      <c r="O34" s="74"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="76"/>
-      <c r="S34" s="74"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="79"/>
+      <c r="S34" s="77"/>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="74"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="77"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="77"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="77"/>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-      <c r="P36" s="74"/>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="76"/>
-      <c r="S36" s="74"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="77"/>
+      <c r="L36" s="77"/>
+      <c r="M36" s="77"/>
+      <c r="N36" s="77"/>
+      <c r="O36" s="77"/>
+      <c r="P36" s="77"/>
+      <c r="Q36" s="77"/>
+      <c r="R36" s="79"/>
+      <c r="S36" s="77"/>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="76"/>
-      <c r="S37" s="74"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="77"/>
+      <c r="L37" s="77"/>
+      <c r="M37" s="77"/>
+      <c r="N37" s="77"/>
+      <c r="O37" s="77"/>
+      <c r="P37" s="77"/>
+      <c r="Q37" s="77"/>
+      <c r="R37" s="79"/>
+      <c r="S37" s="77"/>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="76"/>
-      <c r="S38" s="74"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="78"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="77"/>
+      <c r="O38" s="77"/>
+      <c r="P38" s="77"/>
+      <c r="Q38" s="77"/>
+      <c r="R38" s="79"/>
+      <c r="S38" s="77"/>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="76"/>
-      <c r="S39" s="74"/>
-      <c r="AJ39" s="70"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="78"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="77"/>
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="79"/>
+      <c r="S39" s="77"/>
+      <c r="AJ39" s="73"/>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="74"/>
-      <c r="M40" s="74"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="76"/>
-      <c r="S40" s="74"/>
-      <c r="V40" s="70"/>
-      <c r="W40" s="70"/>
-      <c r="X40" s="70"/>
-      <c r="Y40" s="70"/>
-      <c r="Z40" s="70"/>
-      <c r="AA40" s="70"/>
-      <c r="AB40" s="70"/>
-      <c r="AC40" s="70"/>
-      <c r="AD40" s="70"/>
-      <c r="AE40" s="70"/>
-      <c r="AJ40" s="70"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="78"/>
+      <c r="K40" s="77"/>
+      <c r="L40" s="77"/>
+      <c r="M40" s="77"/>
+      <c r="N40" s="77"/>
+      <c r="O40" s="77"/>
+      <c r="P40" s="77"/>
+      <c r="Q40" s="77"/>
+      <c r="R40" s="79"/>
+      <c r="S40" s="77"/>
+      <c r="V40" s="73"/>
+      <c r="W40" s="73"/>
+      <c r="X40" s="73"/>
+      <c r="Y40" s="73"/>
+      <c r="Z40" s="73"/>
+      <c r="AA40" s="73"/>
+      <c r="AB40" s="73"/>
+      <c r="AC40" s="73"/>
+      <c r="AD40" s="73"/>
+      <c r="AE40" s="73"/>
+      <c r="AJ40" s="73"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="74"/>
-      <c r="M41" s="74"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="76"/>
-      <c r="S41" s="74"/>
-      <c r="V41" s="70"/>
-      <c r="W41" s="70"/>
-      <c r="X41" s="70"/>
-      <c r="Y41" s="70"/>
-      <c r="Z41" s="70"/>
-      <c r="AA41" s="70"/>
-      <c r="AB41" s="70"/>
-      <c r="AC41" s="70"/>
-      <c r="AD41" s="70"/>
-      <c r="AE41" s="70"/>
-      <c r="AJ41" s="70"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="78"/>
+      <c r="K41" s="77"/>
+      <c r="L41" s="77"/>
+      <c r="M41" s="77"/>
+      <c r="N41" s="77"/>
+      <c r="O41" s="77"/>
+      <c r="P41" s="77"/>
+      <c r="Q41" s="77"/>
+      <c r="R41" s="79"/>
+      <c r="S41" s="77"/>
+      <c r="V41" s="73"/>
+      <c r="W41" s="73"/>
+      <c r="X41" s="73"/>
+      <c r="Y41" s="73"/>
+      <c r="Z41" s="73"/>
+      <c r="AA41" s="73"/>
+      <c r="AB41" s="73"/>
+      <c r="AC41" s="73"/>
+      <c r="AD41" s="73"/>
+      <c r="AE41" s="73"/>
+      <c r="AJ41" s="73"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="75"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="76"/>
-      <c r="S42" s="74"/>
-      <c r="V42" s="70"/>
-      <c r="W42" s="70"/>
-      <c r="X42" s="70"/>
-      <c r="Y42" s="70"/>
-      <c r="Z42" s="70"/>
-      <c r="AA42" s="70"/>
-      <c r="AB42" s="70"/>
-      <c r="AC42" s="70"/>
-      <c r="AD42" s="70"/>
-      <c r="AE42" s="70"/>
-      <c r="AJ42" s="70"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="78"/>
+      <c r="K42" s="77"/>
+      <c r="L42" s="77"/>
+      <c r="M42" s="77"/>
+      <c r="N42" s="77"/>
+      <c r="O42" s="77"/>
+      <c r="P42" s="77"/>
+      <c r="Q42" s="77"/>
+      <c r="R42" s="79"/>
+      <c r="S42" s="77"/>
+      <c r="V42" s="73"/>
+      <c r="W42" s="73"/>
+      <c r="X42" s="73"/>
+      <c r="Y42" s="73"/>
+      <c r="Z42" s="73"/>
+      <c r="AA42" s="73"/>
+      <c r="AB42" s="73"/>
+      <c r="AC42" s="73"/>
+      <c r="AD42" s="73"/>
+      <c r="AE42" s="73"/>
+      <c r="AJ42" s="73"/>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="75"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="74"/>
-      <c r="M43" s="74"/>
-      <c r="N43" s="74"/>
-      <c r="O43" s="74"/>
-      <c r="P43" s="74"/>
-      <c r="Q43" s="74"/>
-      <c r="R43" s="76"/>
-      <c r="S43" s="74"/>
-      <c r="V43" s="70"/>
-      <c r="W43" s="70"/>
-      <c r="X43" s="70"/>
-      <c r="Y43" s="70"/>
-      <c r="Z43" s="70"/>
-      <c r="AA43" s="70"/>
-      <c r="AB43" s="70"/>
-      <c r="AC43" s="70"/>
-      <c r="AD43" s="70"/>
-      <c r="AE43" s="70"/>
-      <c r="AJ43" s="70"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="73"/>
+      <c r="J43" s="78"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="77"/>
+      <c r="M43" s="77"/>
+      <c r="N43" s="77"/>
+      <c r="O43" s="77"/>
+      <c r="P43" s="77"/>
+      <c r="Q43" s="77"/>
+      <c r="R43" s="79"/>
+      <c r="S43" s="77"/>
+      <c r="V43" s="73"/>
+      <c r="W43" s="73"/>
+      <c r="X43" s="73"/>
+      <c r="Y43" s="73"/>
+      <c r="Z43" s="73"/>
+      <c r="AA43" s="73"/>
+      <c r="AB43" s="73"/>
+      <c r="AC43" s="73"/>
+      <c r="AD43" s="73"/>
+      <c r="AE43" s="73"/>
+      <c r="AJ43" s="73"/>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="75"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="74"/>
-      <c r="N44" s="74"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="76"/>
-      <c r="S44" s="74"/>
-      <c r="V44" s="70"/>
-      <c r="W44" s="70"/>
-      <c r="X44" s="70"/>
-      <c r="Y44" s="70"/>
-      <c r="Z44" s="70"/>
-      <c r="AA44" s="70"/>
-      <c r="AB44" s="70"/>
-      <c r="AC44" s="70"/>
-      <c r="AD44" s="70"/>
-      <c r="AE44" s="70"/>
-      <c r="AJ44" s="70"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="77"/>
+      <c r="N44" s="77"/>
+      <c r="O44" s="77"/>
+      <c r="P44" s="77"/>
+      <c r="Q44" s="77"/>
+      <c r="R44" s="79"/>
+      <c r="S44" s="77"/>
+      <c r="V44" s="73"/>
+      <c r="W44" s="73"/>
+      <c r="X44" s="73"/>
+      <c r="Y44" s="73"/>
+      <c r="Z44" s="73"/>
+      <c r="AA44" s="73"/>
+      <c r="AB44" s="73"/>
+      <c r="AC44" s="73"/>
+      <c r="AD44" s="73"/>
+      <c r="AE44" s="73"/>
+      <c r="AJ44" s="73"/>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="70"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="74"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="76"/>
-      <c r="S45" s="74"/>
-      <c r="V45" s="70"/>
-      <c r="W45" s="70"/>
-      <c r="X45" s="70"/>
-      <c r="Y45" s="70"/>
-      <c r="Z45" s="70"/>
-      <c r="AA45" s="70"/>
-      <c r="AB45" s="70"/>
-      <c r="AC45" s="70"/>
-      <c r="AD45" s="70"/>
-      <c r="AE45" s="70"/>
-      <c r="AJ45" s="70"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="78"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="77"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="77"/>
+      <c r="P45" s="77"/>
+      <c r="Q45" s="77"/>
+      <c r="R45" s="79"/>
+      <c r="S45" s="77"/>
+      <c r="V45" s="73"/>
+      <c r="W45" s="73"/>
+      <c r="X45" s="73"/>
+      <c r="Y45" s="73"/>
+      <c r="Z45" s="73"/>
+      <c r="AA45" s="73"/>
+      <c r="AB45" s="73"/>
+      <c r="AC45" s="73"/>
+      <c r="AD45" s="73"/>
+      <c r="AE45" s="73"/>
+      <c r="AJ45" s="73"/>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="70"/>
-      <c r="J46" s="75"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-      <c r="M46" s="74"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="74"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="76"/>
-      <c r="S46" s="74"/>
-      <c r="V46" s="70"/>
-      <c r="W46" s="70"/>
-      <c r="X46" s="70"/>
-      <c r="Y46" s="70"/>
-      <c r="Z46" s="70"/>
-      <c r="AA46" s="70"/>
-      <c r="AB46" s="70"/>
-      <c r="AC46" s="70"/>
-      <c r="AD46" s="70"/>
-      <c r="AE46" s="70"/>
-      <c r="AJ46" s="70"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="78"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="77"/>
+      <c r="M46" s="77"/>
+      <c r="N46" s="77"/>
+      <c r="O46" s="77"/>
+      <c r="P46" s="77"/>
+      <c r="Q46" s="77"/>
+      <c r="R46" s="79"/>
+      <c r="S46" s="77"/>
+      <c r="V46" s="73"/>
+      <c r="W46" s="73"/>
+      <c r="X46" s="73"/>
+      <c r="Y46" s="73"/>
+      <c r="Z46" s="73"/>
+      <c r="AA46" s="73"/>
+      <c r="AB46" s="73"/>
+      <c r="AC46" s="73"/>
+      <c r="AD46" s="73"/>
+      <c r="AE46" s="73"/>
+      <c r="AJ46" s="73"/>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="76"/>
-      <c r="S47" s="74"/>
-      <c r="V47" s="70"/>
-      <c r="W47" s="70"/>
-      <c r="X47" s="70"/>
-      <c r="Y47" s="70"/>
-      <c r="Z47" s="70"/>
-      <c r="AA47" s="70"/>
-      <c r="AB47" s="70"/>
-      <c r="AC47" s="70"/>
-      <c r="AD47" s="70"/>
-      <c r="AE47" s="70"/>
-      <c r="AJ47" s="70"/>
+      <c r="F47" s="77"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="73"/>
+      <c r="J47" s="78"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="77"/>
+      <c r="M47" s="77"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="77"/>
+      <c r="P47" s="77"/>
+      <c r="Q47" s="77"/>
+      <c r="R47" s="79"/>
+      <c r="S47" s="77"/>
+      <c r="V47" s="73"/>
+      <c r="W47" s="73"/>
+      <c r="X47" s="73"/>
+      <c r="Y47" s="73"/>
+      <c r="Z47" s="73"/>
+      <c r="AA47" s="73"/>
+      <c r="AB47" s="73"/>
+      <c r="AC47" s="73"/>
+      <c r="AD47" s="73"/>
+      <c r="AE47" s="73"/>
+      <c r="AJ47" s="73"/>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="70"/>
-      <c r="J48" s="75"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="76"/>
-      <c r="S48" s="74"/>
-      <c r="V48" s="70"/>
-      <c r="W48" s="70"/>
-      <c r="X48" s="70"/>
-      <c r="Y48" s="70"/>
-      <c r="Z48" s="70"/>
-      <c r="AA48" s="70"/>
-      <c r="AB48" s="70"/>
-      <c r="AC48" s="70"/>
-      <c r="AD48" s="70"/>
-      <c r="AE48" s="70"/>
-      <c r="AJ48" s="70"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="72"/>
+      <c r="I48" s="73"/>
+      <c r="J48" s="78"/>
+      <c r="K48" s="77"/>
+      <c r="L48" s="77"/>
+      <c r="M48" s="77"/>
+      <c r="N48" s="77"/>
+      <c r="O48" s="77"/>
+      <c r="P48" s="77"/>
+      <c r="Q48" s="77"/>
+      <c r="R48" s="79"/>
+      <c r="S48" s="77"/>
+      <c r="V48" s="73"/>
+      <c r="W48" s="73"/>
+      <c r="X48" s="73"/>
+      <c r="Y48" s="73"/>
+      <c r="Z48" s="73"/>
+      <c r="AA48" s="73"/>
+      <c r="AB48" s="73"/>
+      <c r="AC48" s="73"/>
+      <c r="AD48" s="73"/>
+      <c r="AE48" s="73"/>
+      <c r="AJ48" s="73"/>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="70"/>
-      <c r="J49" s="75"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
-      <c r="M49" s="74"/>
-      <c r="N49" s="74"/>
-      <c r="O49" s="74"/>
-      <c r="P49" s="74"/>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="76"/>
-      <c r="S49" s="74"/>
-      <c r="V49" s="70"/>
-      <c r="W49" s="70"/>
-      <c r="X49" s="70"/>
-      <c r="Y49" s="70"/>
-      <c r="Z49" s="70"/>
-      <c r="AA49" s="70"/>
-      <c r="AB49" s="70"/>
-      <c r="AC49" s="70"/>
-      <c r="AD49" s="70"/>
-      <c r="AE49" s="70"/>
+      <c r="F49" s="77"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="73"/>
+      <c r="J49" s="78"/>
+      <c r="K49" s="77"/>
+      <c r="L49" s="77"/>
+      <c r="M49" s="77"/>
+      <c r="N49" s="77"/>
+      <c r="O49" s="77"/>
+      <c r="P49" s="77"/>
+      <c r="Q49" s="77"/>
+      <c r="R49" s="79"/>
+      <c r="S49" s="77"/>
+      <c r="V49" s="73"/>
+      <c r="W49" s="73"/>
+      <c r="X49" s="73"/>
+      <c r="Y49" s="73"/>
+      <c r="Z49" s="73"/>
+      <c r="AA49" s="73"/>
+      <c r="AB49" s="73"/>
+      <c r="AC49" s="73"/>
+      <c r="AD49" s="73"/>
+      <c r="AE49" s="73"/>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="75"/>
-      <c r="K50" s="74"/>
-      <c r="L50" s="74"/>
-      <c r="M50" s="74"/>
-      <c r="N50" s="74"/>
-      <c r="O50" s="74"/>
-      <c r="P50" s="74"/>
-      <c r="Q50" s="74"/>
-      <c r="R50" s="76"/>
-      <c r="S50" s="74"/>
-      <c r="V50" s="70"/>
-      <c r="W50" s="70"/>
-      <c r="X50" s="70"/>
-      <c r="Y50" s="70"/>
-      <c r="Z50" s="70"/>
-      <c r="AA50" s="70"/>
-      <c r="AB50" s="70"/>
-      <c r="AC50" s="70"/>
-      <c r="AD50" s="70"/>
-      <c r="AE50" s="70"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="77"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="73"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="77"/>
+      <c r="L50" s="77"/>
+      <c r="M50" s="77"/>
+      <c r="N50" s="77"/>
+      <c r="O50" s="77"/>
+      <c r="P50" s="77"/>
+      <c r="Q50" s="77"/>
+      <c r="R50" s="79"/>
+      <c r="S50" s="77"/>
+      <c r="V50" s="73"/>
+      <c r="W50" s="73"/>
+      <c r="X50" s="73"/>
+      <c r="Y50" s="73"/>
+      <c r="Z50" s="73"/>
+      <c r="AA50" s="73"/>
+      <c r="AB50" s="73"/>
+      <c r="AC50" s="73"/>
+      <c r="AD50" s="73"/>
+      <c r="AE50" s="73"/>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F51" s="74"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="70"/>
-      <c r="J51" s="75"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="74"/>
-      <c r="M51" s="74"/>
-      <c r="N51" s="74"/>
-      <c r="O51" s="74"/>
-      <c r="P51" s="74"/>
-      <c r="Q51" s="74"/>
-      <c r="R51" s="76"/>
-      <c r="S51" s="74"/>
-      <c r="V51" s="70"/>
-      <c r="W51" s="70"/>
-      <c r="X51" s="70"/>
-      <c r="Y51" s="70"/>
-      <c r="Z51" s="70"/>
-      <c r="AA51" s="70"/>
-      <c r="AB51" s="70"/>
-      <c r="AC51" s="70"/>
-      <c r="AD51" s="70"/>
-      <c r="AE51" s="70"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="78"/>
+      <c r="K51" s="77"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="77"/>
+      <c r="N51" s="77"/>
+      <c r="O51" s="77"/>
+      <c r="P51" s="77"/>
+      <c r="Q51" s="77"/>
+      <c r="R51" s="79"/>
+      <c r="S51" s="77"/>
+      <c r="V51" s="73"/>
+      <c r="W51" s="73"/>
+      <c r="X51" s="73"/>
+      <c r="Y51" s="73"/>
+      <c r="Z51" s="73"/>
+      <c r="AA51" s="73"/>
+      <c r="AB51" s="73"/>
+      <c r="AC51" s="73"/>
+      <c r="AD51" s="73"/>
+      <c r="AE51" s="73"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="70"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="74"/>
-      <c r="N52" s="74"/>
-      <c r="O52" s="74"/>
-      <c r="P52" s="74"/>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="76"/>
-      <c r="S52" s="74"/>
-      <c r="V52" s="70"/>
-      <c r="W52" s="70"/>
-      <c r="X52" s="70"/>
-      <c r="Y52" s="70"/>
-      <c r="Z52" s="70"/>
-      <c r="AA52" s="70"/>
-      <c r="AB52" s="70"/>
-      <c r="AC52" s="70"/>
-      <c r="AD52" s="70"/>
-      <c r="AE52" s="70"/>
+      <c r="F52" s="77"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="78"/>
+      <c r="K52" s="77"/>
+      <c r="L52" s="77"/>
+      <c r="M52" s="77"/>
+      <c r="N52" s="77"/>
+      <c r="O52" s="77"/>
+      <c r="P52" s="77"/>
+      <c r="Q52" s="77"/>
+      <c r="R52" s="79"/>
+      <c r="S52" s="77"/>
+      <c r="V52" s="73"/>
+      <c r="W52" s="73"/>
+      <c r="X52" s="73"/>
+      <c r="Y52" s="73"/>
+      <c r="Z52" s="73"/>
+      <c r="AA52" s="73"/>
+      <c r="AB52" s="73"/>
+      <c r="AC52" s="73"/>
+      <c r="AD52" s="73"/>
+      <c r="AE52" s="73"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F53" s="74"/>
-      <c r="G53" s="74"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="70"/>
-      <c r="J53" s="75"/>
-      <c r="K53" s="74"/>
-      <c r="L53" s="74"/>
-      <c r="M53" s="74"/>
-      <c r="N53" s="74"/>
-      <c r="O53" s="74"/>
-      <c r="P53" s="74"/>
-      <c r="Q53" s="74"/>
-      <c r="R53" s="76"/>
-      <c r="S53" s="74"/>
-      <c r="V53" s="70"/>
-      <c r="W53" s="70"/>
-      <c r="X53" s="70"/>
-      <c r="Y53" s="70"/>
-      <c r="Z53" s="70"/>
-      <c r="AA53" s="70"/>
-      <c r="AB53" s="70"/>
-      <c r="AC53" s="70"/>
-      <c r="AD53" s="70"/>
-      <c r="AE53" s="70"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="72"/>
+      <c r="I53" s="73"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="77"/>
+      <c r="L53" s="77"/>
+      <c r="M53" s="77"/>
+      <c r="N53" s="77"/>
+      <c r="O53" s="77"/>
+      <c r="P53" s="77"/>
+      <c r="Q53" s="77"/>
+      <c r="R53" s="79"/>
+      <c r="S53" s="77"/>
+      <c r="V53" s="73"/>
+      <c r="W53" s="73"/>
+      <c r="X53" s="73"/>
+      <c r="Y53" s="73"/>
+      <c r="Z53" s="73"/>
+      <c r="AA53" s="73"/>
+      <c r="AB53" s="73"/>
+      <c r="AC53" s="73"/>
+      <c r="AD53" s="73"/>
+      <c r="AE53" s="73"/>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="69"/>
-      <c r="I54" s="70"/>
-      <c r="J54" s="75"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
-      <c r="M54" s="74"/>
-      <c r="N54" s="74"/>
-      <c r="O54" s="74"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
-      <c r="R54" s="76"/>
-      <c r="S54" s="74"/>
-      <c r="V54" s="70"/>
-      <c r="W54" s="70"/>
-      <c r="X54" s="70"/>
-      <c r="Y54" s="70"/>
-      <c r="Z54" s="70"/>
-      <c r="AA54" s="70"/>
-      <c r="AB54" s="70"/>
-      <c r="AC54" s="70"/>
-      <c r="AD54" s="70"/>
-      <c r="AE54" s="70"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="77"/>
+      <c r="L54" s="77"/>
+      <c r="M54" s="77"/>
+      <c r="N54" s="77"/>
+      <c r="O54" s="77"/>
+      <c r="P54" s="77"/>
+      <c r="Q54" s="77"/>
+      <c r="R54" s="79"/>
+      <c r="S54" s="77"/>
+      <c r="V54" s="73"/>
+      <c r="W54" s="73"/>
+      <c r="X54" s="73"/>
+      <c r="Y54" s="73"/>
+      <c r="Z54" s="73"/>
+      <c r="AA54" s="73"/>
+      <c r="AB54" s="73"/>
+      <c r="AC54" s="73"/>
+      <c r="AD54" s="73"/>
+      <c r="AE54" s="73"/>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F55" s="74"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="70"/>
-      <c r="J55" s="75"/>
-      <c r="K55" s="74"/>
-      <c r="L55" s="74"/>
-      <c r="M55" s="74"/>
-      <c r="N55" s="74"/>
-      <c r="O55" s="74"/>
-      <c r="P55" s="74"/>
-      <c r="Q55" s="74"/>
-      <c r="R55" s="76"/>
-      <c r="S55" s="74"/>
-      <c r="V55" s="70"/>
-      <c r="W55" s="70"/>
-      <c r="X55" s="70"/>
-      <c r="Y55" s="70"/>
-      <c r="Z55" s="70"/>
-      <c r="AA55" s="70"/>
-      <c r="AB55" s="70"/>
-      <c r="AC55" s="70"/>
-      <c r="AD55" s="70"/>
-      <c r="AE55" s="70"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="73"/>
+      <c r="J55" s="78"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="77"/>
+      <c r="N55" s="77"/>
+      <c r="O55" s="77"/>
+      <c r="P55" s="77"/>
+      <c r="Q55" s="77"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="77"/>
+      <c r="V55" s="73"/>
+      <c r="W55" s="73"/>
+      <c r="X55" s="73"/>
+      <c r="Y55" s="73"/>
+      <c r="Z55" s="73"/>
+      <c r="AA55" s="73"/>
+      <c r="AB55" s="73"/>
+      <c r="AC55" s="73"/>
+      <c r="AD55" s="73"/>
+      <c r="AE55" s="73"/>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="70"/>
-      <c r="J56" s="75"/>
-      <c r="K56" s="74"/>
-      <c r="L56" s="74"/>
-      <c r="M56" s="74"/>
-      <c r="N56" s="74"/>
-      <c r="O56" s="74"/>
-      <c r="P56" s="74"/>
-      <c r="Q56" s="74"/>
-      <c r="R56" s="76"/>
-      <c r="S56" s="74"/>
-      <c r="V56" s="70"/>
-      <c r="W56" s="70"/>
-      <c r="X56" s="70"/>
-      <c r="Y56" s="70"/>
-      <c r="Z56" s="70"/>
-      <c r="AA56" s="70"/>
-      <c r="AB56" s="70"/>
-      <c r="AC56" s="70"/>
-      <c r="AD56" s="70"/>
-      <c r="AE56" s="70"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="72"/>
+      <c r="I56" s="73"/>
+      <c r="J56" s="78"/>
+      <c r="K56" s="77"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="77"/>
+      <c r="N56" s="77"/>
+      <c r="O56" s="77"/>
+      <c r="P56" s="77"/>
+      <c r="Q56" s="77"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="77"/>
+      <c r="V56" s="73"/>
+      <c r="W56" s="73"/>
+      <c r="X56" s="73"/>
+      <c r="Y56" s="73"/>
+      <c r="Z56" s="73"/>
+      <c r="AA56" s="73"/>
+      <c r="AB56" s="73"/>
+      <c r="AC56" s="73"/>
+      <c r="AD56" s="73"/>
+      <c r="AE56" s="73"/>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F57" s="74"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="74"/>
-      <c r="K57" s="74"/>
-      <c r="L57" s="74"/>
-      <c r="M57" s="74"/>
-      <c r="N57" s="74"/>
-      <c r="O57" s="74"/>
-      <c r="P57" s="74"/>
-      <c r="Q57" s="74"/>
-      <c r="R57" s="76"/>
-      <c r="S57" s="74"/>
-      <c r="V57" s="70"/>
-      <c r="W57" s="70"/>
-      <c r="X57" s="70"/>
-      <c r="Y57" s="70"/>
-      <c r="Z57" s="70"/>
-      <c r="AA57" s="70"/>
-      <c r="AB57" s="70"/>
-      <c r="AC57" s="70"/>
-      <c r="AD57" s="70"/>
-      <c r="AE57" s="70"/>
+      <c r="F57" s="77"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="80"/>
+      <c r="J57" s="77"/>
+      <c r="K57" s="77"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="77"/>
+      <c r="N57" s="77"/>
+      <c r="O57" s="77"/>
+      <c r="P57" s="77"/>
+      <c r="Q57" s="77"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="77"/>
+      <c r="V57" s="73"/>
+      <c r="W57" s="73"/>
+      <c r="X57" s="73"/>
+      <c r="Y57" s="73"/>
+      <c r="Z57" s="73"/>
+      <c r="AA57" s="73"/>
+      <c r="AB57" s="73"/>
+      <c r="AC57" s="73"/>
+      <c r="AD57" s="73"/>
+      <c r="AE57" s="73"/>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H58" s="70"/>
-      <c r="I58" s="70"/>
-      <c r="J58" s="75"/>
-      <c r="K58" s="74"/>
-      <c r="L58" s="74"/>
-      <c r="M58" s="74"/>
-      <c r="N58" s="74"/>
-      <c r="O58" s="74"/>
-      <c r="P58" s="74"/>
-      <c r="Q58" s="74"/>
-      <c r="R58" s="76"/>
-      <c r="S58" s="74"/>
-      <c r="V58" s="70"/>
-      <c r="W58" s="70"/>
-      <c r="X58" s="70"/>
-      <c r="Y58" s="70"/>
-      <c r="Z58" s="70"/>
-      <c r="AA58" s="70"/>
-      <c r="AB58" s="70"/>
-      <c r="AC58" s="70"/>
-      <c r="AD58" s="70"/>
-      <c r="AE58" s="70"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="78"/>
+      <c r="K58" s="77"/>
+      <c r="L58" s="77"/>
+      <c r="M58" s="77"/>
+      <c r="N58" s="77"/>
+      <c r="O58" s="77"/>
+      <c r="P58" s="77"/>
+      <c r="Q58" s="77"/>
+      <c r="R58" s="79"/>
+      <c r="S58" s="77"/>
+      <c r="V58" s="73"/>
+      <c r="W58" s="73"/>
+      <c r="X58" s="73"/>
+      <c r="Y58" s="73"/>
+      <c r="Z58" s="73"/>
+      <c r="AA58" s="73"/>
+      <c r="AB58" s="73"/>
+      <c r="AC58" s="73"/>
+      <c r="AD58" s="73"/>
+      <c r="AE58" s="73"/>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="70"/>
-      <c r="I59" s="70"/>
-      <c r="J59" s="75"/>
-      <c r="K59" s="74"/>
-      <c r="L59" s="74"/>
-      <c r="M59" s="74"/>
-      <c r="N59" s="74"/>
-      <c r="O59" s="74"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="74"/>
-      <c r="R59" s="76"/>
-      <c r="S59" s="74"/>
-      <c r="V59" s="70"/>
-      <c r="W59" s="70"/>
-      <c r="X59" s="70"/>
-      <c r="Y59" s="70"/>
-      <c r="Z59" s="70"/>
-      <c r="AA59" s="70"/>
-      <c r="AB59" s="70"/>
-      <c r="AC59" s="70"/>
-      <c r="AD59" s="70"/>
-      <c r="AE59" s="70"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="78"/>
+      <c r="K59" s="77"/>
+      <c r="L59" s="77"/>
+      <c r="M59" s="77"/>
+      <c r="N59" s="77"/>
+      <c r="O59" s="77"/>
+      <c r="P59" s="77"/>
+      <c r="Q59" s="77"/>
+      <c r="R59" s="79"/>
+      <c r="S59" s="77"/>
+      <c r="V59" s="73"/>
+      <c r="W59" s="73"/>
+      <c r="X59" s="73"/>
+      <c r="Y59" s="73"/>
+      <c r="Z59" s="73"/>
+      <c r="AA59" s="73"/>
+      <c r="AB59" s="73"/>
+      <c r="AC59" s="73"/>
+      <c r="AD59" s="73"/>
+      <c r="AE59" s="73"/>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
-      <c r="J60" s="78"/>
-      <c r="K60" s="79"/>
-      <c r="L60" s="79"/>
-      <c r="M60" s="79"/>
-      <c r="N60" s="79"/>
-      <c r="O60" s="79"/>
-      <c r="P60" s="79"/>
-      <c r="Q60" s="79"/>
-      <c r="R60" s="80"/>
-      <c r="S60" s="74"/>
-      <c r="V60" s="70"/>
-      <c r="W60" s="70"/>
-      <c r="X60" s="70"/>
-      <c r="Y60" s="70"/>
-      <c r="Z60" s="70"/>
-      <c r="AA60" s="70"/>
-      <c r="AB60" s="70"/>
-      <c r="AC60" s="70"/>
-      <c r="AD60" s="70"/>
-      <c r="AE60" s="70"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="81"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="82"/>
+      <c r="N60" s="82"/>
+      <c r="O60" s="82"/>
+      <c r="P60" s="82"/>
+      <c r="Q60" s="82"/>
+      <c r="R60" s="83"/>
+      <c r="S60" s="77"/>
+      <c r="V60" s="73"/>
+      <c r="W60" s="73"/>
+      <c r="X60" s="73"/>
+      <c r="Y60" s="73"/>
+      <c r="Z60" s="73"/>
+      <c r="AA60" s="73"/>
+      <c r="AB60" s="73"/>
+      <c r="AC60" s="73"/>
+      <c r="AD60" s="73"/>
+      <c r="AE60" s="73"/>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V61" s="70"/>
-      <c r="W61" s="70"/>
-      <c r="X61" s="70"/>
-      <c r="Y61" s="70"/>
-      <c r="Z61" s="70"/>
-      <c r="AA61" s="70"/>
-      <c r="AB61" s="70"/>
-      <c r="AC61" s="70"/>
-      <c r="AD61" s="70"/>
-      <c r="AE61" s="70"/>
+      <c r="V61" s="73"/>
+      <c r="W61" s="73"/>
+      <c r="X61" s="73"/>
+      <c r="Y61" s="73"/>
+      <c r="Z61" s="73"/>
+      <c r="AA61" s="73"/>
+      <c r="AB61" s="73"/>
+      <c r="AC61" s="73"/>
+      <c r="AD61" s="73"/>
+      <c r="AE61" s="73"/>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V62" s="70"/>
-      <c r="W62" s="70"/>
-      <c r="X62" s="70"/>
-      <c r="Y62" s="70"/>
-      <c r="Z62" s="70"/>
-      <c r="AA62" s="70"/>
-      <c r="AB62" s="70"/>
-      <c r="AC62" s="70"/>
-      <c r="AD62" s="70"/>
-      <c r="AE62" s="70"/>
+      <c r="V62" s="73"/>
+      <c r="W62" s="73"/>
+      <c r="X62" s="73"/>
+      <c r="Y62" s="73"/>
+      <c r="Z62" s="73"/>
+      <c r="AA62" s="73"/>
+      <c r="AB62" s="73"/>
+      <c r="AC62" s="73"/>
+      <c r="AD62" s="73"/>
+      <c r="AE62" s="73"/>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V63" s="70"/>
-      <c r="W63" s="70"/>
-      <c r="X63" s="70"/>
-      <c r="Y63" s="70"/>
-      <c r="Z63" s="70"/>
-      <c r="AA63" s="70"/>
-      <c r="AB63" s="70"/>
-      <c r="AC63" s="70"/>
-      <c r="AD63" s="70"/>
-      <c r="AE63" s="70"/>
+      <c r="V63" s="73"/>
+      <c r="W63" s="73"/>
+      <c r="X63" s="73"/>
+      <c r="Y63" s="73"/>
+      <c r="Z63" s="73"/>
+      <c r="AA63" s="73"/>
+      <c r="AB63" s="73"/>
+      <c r="AC63" s="73"/>
+      <c r="AD63" s="73"/>
+      <c r="AE63" s="73"/>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V64" s="70"/>
-      <c r="W64" s="70"/>
-      <c r="X64" s="70"/>
-      <c r="Y64" s="70"/>
-      <c r="Z64" s="70"/>
-      <c r="AA64" s="70"/>
-      <c r="AB64" s="70"/>
-      <c r="AC64" s="70"/>
-      <c r="AD64" s="70"/>
-      <c r="AE64" s="70"/>
+      <c r="V64" s="73"/>
+      <c r="W64" s="73"/>
+      <c r="X64" s="73"/>
+      <c r="Y64" s="73"/>
+      <c r="Z64" s="73"/>
+      <c r="AA64" s="73"/>
+      <c r="AB64" s="73"/>
+      <c r="AC64" s="73"/>
+      <c r="AD64" s="73"/>
+      <c r="AE64" s="73"/>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V65" s="70"/>
-      <c r="W65" s="70"/>
-      <c r="X65" s="70"/>
-      <c r="Y65" s="70"/>
-      <c r="Z65" s="70"/>
-      <c r="AA65" s="70"/>
-      <c r="AB65" s="70"/>
-      <c r="AC65" s="70"/>
-      <c r="AD65" s="70"/>
-      <c r="AE65" s="70"/>
+      <c r="V65" s="73"/>
+      <c r="W65" s="73"/>
+      <c r="X65" s="73"/>
+      <c r="Y65" s="73"/>
+      <c r="Z65" s="73"/>
+      <c r="AA65" s="73"/>
+      <c r="AB65" s="73"/>
+      <c r="AC65" s="73"/>
+      <c r="AD65" s="73"/>
+      <c r="AE65" s="73"/>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V66" s="70"/>
-      <c r="W66" s="70"/>
-      <c r="X66" s="70"/>
-      <c r="Y66" s="70"/>
-      <c r="Z66" s="70"/>
-      <c r="AA66" s="70"/>
-      <c r="AB66" s="70"/>
-      <c r="AC66" s="70"/>
-      <c r="AD66" s="70"/>
-      <c r="AE66" s="70"/>
+      <c r="V66" s="73"/>
+      <c r="W66" s="73"/>
+      <c r="X66" s="73"/>
+      <c r="Y66" s="73"/>
+      <c r="Z66" s="73"/>
+      <c r="AA66" s="73"/>
+      <c r="AB66" s="73"/>
+      <c r="AC66" s="73"/>
+      <c r="AD66" s="73"/>
+      <c r="AE66" s="73"/>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V67" s="70"/>
-      <c r="W67" s="70"/>
-      <c r="X67" s="70"/>
-      <c r="Y67" s="70"/>
-      <c r="Z67" s="70"/>
-      <c r="AA67" s="70"/>
-      <c r="AB67" s="70"/>
-      <c r="AC67" s="70"/>
-      <c r="AD67" s="70"/>
-      <c r="AE67" s="70"/>
+      <c r="V67" s="73"/>
+      <c r="W67" s="73"/>
+      <c r="X67" s="73"/>
+      <c r="Y67" s="73"/>
+      <c r="Z67" s="73"/>
+      <c r="AA67" s="73"/>
+      <c r="AB67" s="73"/>
+      <c r="AC67" s="73"/>
+      <c r="AD67" s="73"/>
+      <c r="AE67" s="73"/>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V68" s="70"/>
-      <c r="W68" s="70"/>
-      <c r="X68" s="70"/>
-      <c r="Y68" s="70"/>
-      <c r="Z68" s="70"/>
-      <c r="AA68" s="70"/>
-      <c r="AB68" s="70"/>
-      <c r="AC68" s="70"/>
-      <c r="AD68" s="70"/>
-      <c r="AE68" s="70"/>
+      <c r="V68" s="73"/>
+      <c r="W68" s="73"/>
+      <c r="X68" s="73"/>
+      <c r="Y68" s="73"/>
+      <c r="Z68" s="73"/>
+      <c r="AA68" s="73"/>
+      <c r="AB68" s="73"/>
+      <c r="AC68" s="73"/>
+      <c r="AD68" s="73"/>
+      <c r="AE68" s="73"/>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V69" s="70"/>
-      <c r="W69" s="70"/>
-      <c r="X69" s="70"/>
-      <c r="Y69" s="70"/>
-      <c r="Z69" s="70"/>
-      <c r="AA69" s="70"/>
-      <c r="AB69" s="70"/>
-      <c r="AC69" s="70"/>
-      <c r="AD69" s="70"/>
-      <c r="AE69" s="70"/>
+      <c r="V69" s="73"/>
+      <c r="W69" s="73"/>
+      <c r="X69" s="73"/>
+      <c r="Y69" s="73"/>
+      <c r="Z69" s="73"/>
+      <c r="AA69" s="73"/>
+      <c r="AB69" s="73"/>
+      <c r="AC69" s="73"/>
+      <c r="AD69" s="73"/>
+      <c r="AE69" s="73"/>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V70" s="70"/>
-      <c r="W70" s="70"/>
-      <c r="X70" s="70"/>
-      <c r="Y70" s="70"/>
-      <c r="Z70" s="70"/>
-      <c r="AA70" s="70"/>
-      <c r="AB70" s="70"/>
-      <c r="AC70" s="70"/>
-      <c r="AD70" s="70"/>
-      <c r="AE70" s="70"/>
+      <c r="V70" s="73"/>
+      <c r="W70" s="73"/>
+      <c r="X70" s="73"/>
+      <c r="Y70" s="73"/>
+      <c r="Z70" s="73"/>
+      <c r="AA70" s="73"/>
+      <c r="AB70" s="73"/>
+      <c r="AC70" s="73"/>
+      <c r="AD70" s="73"/>
+      <c r="AE70" s="73"/>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V71" s="70"/>
-      <c r="W71" s="70"/>
-      <c r="X71" s="70"/>
-      <c r="Y71" s="70"/>
-      <c r="Z71" s="70"/>
-      <c r="AA71" s="70"/>
-      <c r="AB71" s="70"/>
-      <c r="AC71" s="70"/>
-      <c r="AD71" s="70"/>
-      <c r="AE71" s="70"/>
+      <c r="V71" s="73"/>
+      <c r="W71" s="73"/>
+      <c r="X71" s="73"/>
+      <c r="Y71" s="73"/>
+      <c r="Z71" s="73"/>
+      <c r="AA71" s="73"/>
+      <c r="AB71" s="73"/>
+      <c r="AC71" s="73"/>
+      <c r="AD71" s="73"/>
+      <c r="AE71" s="73"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="true"/>

</xml_diff>